<commit_message>
Agregue la columna Event_M con los datos modificados a pedido de Laura y Dario. DS es duda smoke. DN duda con tendencia a la negativa.
</commit_message>
<xml_diff>
--- a/BA_events_test.xlsx
+++ b/BA_events_test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="55">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -35,16 +35,25 @@
     <t xml:space="preserve">Event</t>
   </si>
   <si>
+    <t xml:space="preserve">Event_M</t>
+  </si>
+  <si>
     <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">SN</t>
   </si>
   <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS</t>
+  </si>
+  <si>
     <t xml:space="preserve">SP</t>
   </si>
   <si>
-    <t xml:space="preserve">S</t>
+    <t xml:space="preserve">DN</t>
   </si>
   <si>
     <t xml:space="preserve">chek</t>
@@ -447,23 +456,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
-      <selection pane="bottomRight" activeCell="F72" activeCellId="0" sqref="F72"/>
+      <selection pane="bottomLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="10.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,8 +483,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>43558</v>
       </c>
@@ -488,10 +498,13 @@
         <v>0.509858807017544</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>43561</v>
       </c>
@@ -502,10 +515,13 @@
         <v>0.499241586956522</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>43564</v>
       </c>
@@ -516,10 +532,13 @@
         <v>0.7347548</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>43567</v>
       </c>
@@ -530,10 +549,13 @@
         <v>1.19260968316832</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>43570</v>
       </c>
@@ -544,10 +566,13 @@
         <v>0.43373725</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>43573</v>
       </c>
@@ -558,10 +583,13 @@
         <v>1.03454433333333</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>43576</v>
       </c>
@@ -572,10 +600,13 @@
         <v>1.0762931</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>43579</v>
       </c>
@@ -586,10 +617,13 @@
         <v>1.0368655</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>43582</v>
       </c>
@@ -600,10 +634,13 @@
         <v>0.510182083333333</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>43585</v>
       </c>
@@ -614,10 +651,13 @@
         <v>0.628600555555556</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>43588</v>
       </c>
@@ -628,10 +668,13 @@
         <v>0.702352763888889</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>43591</v>
       </c>
@@ -642,10 +685,13 @@
         <v>0.842384479452055</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>43597</v>
       </c>
@@ -656,10 +702,13 @@
         <v>1.17002332352941</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>43600</v>
       </c>
@@ -670,10 +719,13 @@
         <v>0.247635011560694</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>43603</v>
       </c>
@@ -684,10 +736,13 @@
         <v>1.05060265217391</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>43609</v>
       </c>
@@ -698,10 +753,13 @@
         <v>1.06950337704918</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>43612</v>
       </c>
@@ -712,20 +770,26 @@
         <v>0.878866545905707</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>43615</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>43618</v>
       </c>
@@ -736,7 +800,10 @@
         <v>1.50325183333333</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -746,6 +813,9 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -754,6 +824,9 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -762,6 +835,9 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -774,6 +850,9 @@
         <v>0.337774125</v>
       </c>
       <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -782,7 +861,10 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -792,6 +874,9 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -800,6 +885,9 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -812,7 +900,10 @@
         <v>1.24706230612245</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -822,7 +913,10 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -838,6 +932,9 @@
       <c r="D30" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E30" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -850,7 +947,10 @@
         <v>1.57611228571429</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -862,6 +962,9 @@
       <c r="D32" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E32" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -870,6 +973,9 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
@@ -878,6 +984,9 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -890,7 +999,10 @@
         <v>1.212169</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -904,7 +1016,10 @@
         <v>0.43259440625</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -918,7 +1033,10 @@
         <v>0.981173706349207</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -934,6 +1052,9 @@
       <c r="D38" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E38" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -946,7 +1067,10 @@
         <v>0.891150205479452</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -960,7 +1084,10 @@
         <v>1.02793206896552</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -976,6 +1103,9 @@
       <c r="D41" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E41" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -988,7 +1118,10 @@
         <v>0.86211475</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1004,6 +1137,9 @@
       <c r="D43" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E43" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
@@ -1016,6 +1152,9 @@
         <v>1.516236</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1028,6 +1167,9 @@
       <c r="D45" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E45" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
@@ -1040,7 +1182,10 @@
         <v>1.1401608137931</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1054,7 +1199,10 @@
         <v>0.688018344827586</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1064,7 +1212,10 @@
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1074,7 +1225,10 @@
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1088,7 +1242,10 @@
         <v>1.26060492763158</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1104,6 +1261,9 @@
       <c r="D51" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E51" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
@@ -1116,7 +1276,10 @@
         <v>0.966215441860465</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1130,7 +1293,10 @@
         <v>0.600562924731183</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1144,7 +1310,10 @@
         <v>0.983993447368421</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1158,7 +1327,10 @@
         <v>1.046564</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1174,6 +1346,9 @@
       <c r="D56" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E56" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
@@ -1182,6 +1357,9 @@
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
@@ -1194,7 +1372,10 @@
         <v>1.43679937951807</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1208,7 +1389,10 @@
         <v>1.02183162962963</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1218,6 +1402,9 @@
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
+      <c r="E60" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
@@ -1230,7 +1417,10 @@
         <v>0.961475944099378</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1246,6 +1436,9 @@
       <c r="D62" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E62" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
@@ -1258,7 +1451,10 @@
         <v>0.770984827338129</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1268,6 +1464,9 @@
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
@@ -1280,7 +1479,10 @@
         <v>0.900937777777778</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1294,7 +1496,10 @@
         <v>0.772298905660378</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1308,7 +1513,10 @@
         <v>0.642724304347826</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1324,6 +1532,9 @@
       <c r="D68" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E68" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
@@ -1336,7 +1547,10 @@
         <v>1.03860773529412</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1352,6 +1566,9 @@
       <c r="D70" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E70" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
@@ -1364,7 +1581,10 @@
         <v>1.29882684615385</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1380,6 +1600,9 @@
       <c r="D72" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E72" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
@@ -1392,7 +1615,10 @@
         <v>0.526924511450382</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1406,7 +1632,10 @@
         <v>1.15243975</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1420,7 +1649,10 @@
         <v>1.01949652380952</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1434,7 +1666,10 @@
         <v>1.03208732620321</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1448,7 +1683,10 @@
         <v>1.01991402649007</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1462,7 +1700,10 @@
         <v>1.02417112658228</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1478,6 +1719,9 @@
       <c r="D79" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E79" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
@@ -1490,7 +1734,10 @@
         <v>0.877221</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1504,7 +1751,10 @@
         <v>1.30902159134615</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1514,7 +1764,10 @@
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1528,7 +1781,10 @@
         <v>0.7380234</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1542,6 +1798,9 @@
         <v>0.652622229508197</v>
       </c>
       <c r="D84" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1558,6 +1817,9 @@
       <c r="D85" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E85" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
@@ -1572,6 +1834,9 @@
       <c r="D86" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E86" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
@@ -1586,6 +1851,9 @@
       <c r="D87" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E87" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
@@ -1600,6 +1868,9 @@
       <c r="D88" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E88" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
@@ -1614,6 +1885,9 @@
       <c r="D89" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E89" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
@@ -1628,6 +1902,9 @@
       <c r="D90" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E90" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
@@ -1636,6 +1913,9 @@
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
+      <c r="E91" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
@@ -1648,7 +1928,10 @@
         <v>0.983014304694423</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1662,7 +1945,10 @@
         <v>0.987089936893204</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1678,6 +1964,9 @@
       <c r="D94" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E94" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
@@ -1690,7 +1979,10 @@
         <v>0.787264</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1704,7 +1996,10 @@
         <v>1.14074691752577</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1718,7 +2013,10 @@
         <v>0.781452411764706</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1732,7 +2030,10 @@
         <v>0.44478180952381</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1746,7 +2047,10 @@
         <v>1.23533518699187</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1756,6 +2060,9 @@
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
+      <c r="E100" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="n">
@@ -1768,7 +2075,10 @@
         <v>1.17759195402299</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4470,8 +4780,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4494,7 +4804,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="1" style="0" width="10.86"/>
   </cols>
@@ -4504,133 +4814,133 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AE1" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="AF1" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AH1" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AI1" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AJ1" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AK1" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AL1" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AM1" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AN1" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="AO1" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="AQ1" s="9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AR1" s="9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18935,8 +19245,8 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>